<commit_message>
update the html template
</commit_message>
<xml_diff>
--- a/Data/MarginFileClalOnlyApril2017.xlsx
+++ b/Data/MarginFileClalOnlyApril2017.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18201"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -566,15 +566,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AC188"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="M99" sqref="M99"/>
+    <sheetView tabSelected="1" topLeftCell="A130" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C145" sqref="C145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23.44140625" customWidth="1"/>
-    <col min="2" max="2" width="6.44140625" style="5" customWidth="1"/>
-    <col min="3" max="29" width="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="29" width="7.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:29" s="5" customFormat="1" x14ac:dyDescent="0.3">
@@ -13483,537 +13483,537 @@
       </c>
     </row>
     <row r="146" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A146" t="s">
+      <c r="A146" s="11" t="s">
         <v>24</v>
       </c>
       <c r="B146" s="6">
         <v>1</v>
       </c>
-      <c r="C146" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="D146" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="E146" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="F146" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="G146" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="H146" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="I146" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="J146" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="K146" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="L146" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="M146" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="N146" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="O146" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="P146" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="Q146" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="R146" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="S146" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="T146" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="U146" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="V146" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="W146" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="X146" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="Y146" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="Z146" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="AA146" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="AB146" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="AC146" s="10">
-        <v>-0.01</v>
+      <c r="C146" s="13">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="D146" s="13">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="E146" s="13">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="F146" s="13">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="G146" s="13">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="H146" s="13">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="I146" s="13">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="J146" s="13">
+        <v>4.1999999999999997E-3</v>
+      </c>
+      <c r="K146" s="13">
+        <v>4.1999999999999997E-3</v>
+      </c>
+      <c r="L146" s="13">
+        <v>4.1999999999999997E-3</v>
+      </c>
+      <c r="M146" s="13">
+        <v>4.1999999999999997E-3</v>
+      </c>
+      <c r="N146" s="13">
+        <v>4.1999999999999997E-3</v>
+      </c>
+      <c r="O146" s="13">
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="P146" s="13">
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="Q146" s="13">
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="R146" s="13">
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="S146" s="13">
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="T146" s="13">
+        <v>4.7999999999999996E-3</v>
+      </c>
+      <c r="U146" s="13">
+        <v>4.7999999999999996E-3</v>
+      </c>
+      <c r="V146" s="13">
+        <v>4.7999999999999996E-3</v>
+      </c>
+      <c r="W146" s="13">
+        <v>4.7999999999999996E-3</v>
+      </c>
+      <c r="X146" s="13">
+        <v>4.7999999999999996E-3</v>
+      </c>
+      <c r="Y146" s="13">
+        <v>5.1999999999999998E-3</v>
+      </c>
+      <c r="Z146" s="13">
+        <v>5.1999999999999998E-3</v>
+      </c>
+      <c r="AA146" s="13">
+        <v>5.1999999999999998E-3</v>
+      </c>
+      <c r="AB146" s="13">
+        <v>5.1999999999999998E-3</v>
+      </c>
+      <c r="AC146" s="13">
+        <v>5.1999999999999998E-3</v>
       </c>
     </row>
     <row r="147" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A147" t="s">
+      <c r="A147" s="11" t="s">
         <v>24</v>
       </c>
       <c r="B147" s="7">
         <v>2</v>
       </c>
-      <c r="C147" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="D147" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="E147" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="F147" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="G147" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="H147" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="I147" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="J147" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="K147" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="L147" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="M147" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="N147" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="O147" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="P147" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="Q147" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="R147" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="S147" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="T147" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="U147" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="V147" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="W147" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="X147" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="Y147" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="Z147" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="AA147" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="AB147" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="AC147" s="10">
-        <v>-0.01</v>
+      <c r="C147" s="13">
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="D147" s="13">
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="E147" s="13">
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="F147" s="13">
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="G147" s="13">
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="H147" s="13">
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="I147" s="13">
+        <v>4.4999999999999997E-3</v>
+      </c>
+      <c r="J147" s="13">
+        <v>4.7999999999999996E-3</v>
+      </c>
+      <c r="K147" s="13">
+        <v>4.7999999999999996E-3</v>
+      </c>
+      <c r="L147" s="13">
+        <v>4.7999999999999996E-3</v>
+      </c>
+      <c r="M147" s="13">
+        <v>4.7999999999999996E-3</v>
+      </c>
+      <c r="N147" s="13">
+        <v>4.7999999999999996E-3</v>
+      </c>
+      <c r="O147" s="13">
+        <v>5.1999999999999998E-3</v>
+      </c>
+      <c r="P147" s="13">
+        <v>5.1999999999999998E-3</v>
+      </c>
+      <c r="Q147" s="13">
+        <v>5.1999999999999998E-3</v>
+      </c>
+      <c r="R147" s="13">
+        <v>5.1999999999999998E-3</v>
+      </c>
+      <c r="S147" s="13">
+        <v>5.1999999999999998E-3</v>
+      </c>
+      <c r="T147" s="13">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="U147" s="13">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="V147" s="13">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="W147" s="13">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="X147" s="13">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="Y147" s="13">
+        <v>5.8999999999999999E-3</v>
+      </c>
+      <c r="Z147" s="13">
+        <v>5.8999999999999999E-3</v>
+      </c>
+      <c r="AA147" s="13">
+        <v>5.8999999999999999E-3</v>
+      </c>
+      <c r="AB147" s="13">
+        <v>5.8999999999999999E-3</v>
+      </c>
+      <c r="AC147" s="13">
+        <v>5.8999999999999999E-3</v>
       </c>
     </row>
     <row r="148" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A148" t="s">
+      <c r="A148" s="11" t="s">
         <v>24</v>
       </c>
       <c r="B148" s="7">
         <v>3</v>
       </c>
-      <c r="C148" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="D148" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="E148" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="F148" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="G148" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="H148" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="I148" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="J148" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="K148" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="L148" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="M148" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="N148" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="O148" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="P148" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="Q148" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="R148" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="S148" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="T148" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="U148" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="V148" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="W148" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="X148" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="Y148" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="Z148" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="AA148" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="AB148" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="AC148" s="10">
-        <v>-0.01</v>
+      <c r="C148" s="13">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D148" s="13">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E148" s="13">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="F148" s="13">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="G148" s="13">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="H148" s="13">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="I148" s="13">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="J148" s="13">
+        <v>5.4000000000000003E-3</v>
+      </c>
+      <c r="K148" s="13">
+        <v>5.4000000000000003E-3</v>
+      </c>
+      <c r="L148" s="13">
+        <v>5.4000000000000003E-3</v>
+      </c>
+      <c r="M148" s="13">
+        <v>5.4000000000000003E-3</v>
+      </c>
+      <c r="N148" s="13">
+        <v>5.4000000000000003E-3</v>
+      </c>
+      <c r="O148" s="13">
+        <v>5.7999999999999996E-3</v>
+      </c>
+      <c r="P148" s="13">
+        <v>5.7999999999999996E-3</v>
+      </c>
+      <c r="Q148" s="13">
+        <v>5.7999999999999996E-3</v>
+      </c>
+      <c r="R148" s="13">
+        <v>5.7999999999999996E-3</v>
+      </c>
+      <c r="S148" s="13">
+        <v>5.7999999999999996E-3</v>
+      </c>
+      <c r="T148" s="13">
+        <v>6.1999999999999998E-3</v>
+      </c>
+      <c r="U148" s="13">
+        <v>6.1999999999999998E-3</v>
+      </c>
+      <c r="V148" s="13">
+        <v>6.1999999999999998E-3</v>
+      </c>
+      <c r="W148" s="13">
+        <v>6.1999999999999998E-3</v>
+      </c>
+      <c r="X148" s="13">
+        <v>6.1999999999999998E-3</v>
+      </c>
+      <c r="Y148" s="13">
+        <v>6.7999999999999996E-3</v>
+      </c>
+      <c r="Z148" s="13">
+        <v>6.7999999999999996E-3</v>
+      </c>
+      <c r="AA148" s="13">
+        <v>6.7999999999999996E-3</v>
+      </c>
+      <c r="AB148" s="13">
+        <v>6.7999999999999996E-3</v>
+      </c>
+      <c r="AC148" s="13">
+        <v>6.7999999999999996E-3</v>
       </c>
     </row>
     <row r="149" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A149" t="s">
+      <c r="A149" s="11" t="s">
         <v>24</v>
       </c>
       <c r="B149" s="7">
         <v>4</v>
       </c>
-      <c r="C149" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="D149" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="E149" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="F149" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="G149" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="H149" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="I149" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="J149" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="K149" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="L149" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="M149" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="N149" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="O149" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="P149" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="Q149" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="R149" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="S149" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="T149" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="U149" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="V149" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="W149" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="X149" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="Y149" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="Z149" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="AA149" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="AB149" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="AC149" s="10">
-        <v>-0.01</v>
+      <c r="C149" s="13">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="D149" s="13">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="E149" s="13">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="F149" s="13">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="G149" s="13">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="H149" s="13">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="I149" s="13">
+        <v>5.4999999999999997E-3</v>
+      </c>
+      <c r="J149" s="13">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="K149" s="13">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="L149" s="13">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="M149" s="13">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="N149" s="13">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="O149" s="13">
+        <v>6.6E-3</v>
+      </c>
+      <c r="P149" s="13">
+        <v>6.6E-3</v>
+      </c>
+      <c r="Q149" s="13">
+        <v>6.6E-3</v>
+      </c>
+      <c r="R149" s="13">
+        <v>6.6E-3</v>
+      </c>
+      <c r="S149" s="13">
+        <v>6.6E-3</v>
+      </c>
+      <c r="T149" s="13">
+        <v>6.8999999999999999E-3</v>
+      </c>
+      <c r="U149" s="13">
+        <v>6.8999999999999999E-3</v>
+      </c>
+      <c r="V149" s="13">
+        <v>6.8999999999999999E-3</v>
+      </c>
+      <c r="W149" s="13">
+        <v>6.8999999999999999E-3</v>
+      </c>
+      <c r="X149" s="13">
+        <v>6.8999999999999999E-3</v>
+      </c>
+      <c r="Y149" s="13">
+        <v>7.7999999999999996E-3</v>
+      </c>
+      <c r="Z149" s="13">
+        <v>7.7999999999999996E-3</v>
+      </c>
+      <c r="AA149" s="13">
+        <v>7.7999999999999996E-3</v>
+      </c>
+      <c r="AB149" s="13">
+        <v>7.7999999999999996E-3</v>
+      </c>
+      <c r="AC149" s="13">
+        <v>7.7999999999999996E-3</v>
       </c>
     </row>
     <row r="150" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A150" t="s">
+      <c r="A150" s="11" t="s">
         <v>24</v>
       </c>
       <c r="B150" s="7">
         <v>5</v>
       </c>
-      <c r="C150" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="D150" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="E150" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="F150" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="G150" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="H150" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="I150" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="J150" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="K150" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="L150" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="M150" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="N150" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="O150" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="P150" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="Q150" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="R150" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="S150" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="T150" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="U150" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="V150" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="W150" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="X150" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="Y150" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="Z150" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="AA150" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="AB150" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="AC150" s="10">
-        <v>-0.01</v>
+      <c r="C150" s="13">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D150" s="13">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="E150" s="13">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="F150" s="13">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="G150" s="13">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="H150" s="13">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="I150" s="13">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="J150" s="13">
+        <v>6.4999999999999997E-3</v>
+      </c>
+      <c r="K150" s="13">
+        <v>6.4999999999999997E-3</v>
+      </c>
+      <c r="L150" s="13">
+        <v>6.4999999999999997E-3</v>
+      </c>
+      <c r="M150" s="13">
+        <v>6.4999999999999997E-3</v>
+      </c>
+      <c r="N150" s="13">
+        <v>6.4999999999999997E-3</v>
+      </c>
+      <c r="O150" s="13">
+        <v>7.1000000000000004E-3</v>
+      </c>
+      <c r="P150" s="13">
+        <v>7.1000000000000004E-3</v>
+      </c>
+      <c r="Q150" s="13">
+        <v>7.1000000000000004E-3</v>
+      </c>
+      <c r="R150" s="13">
+        <v>7.1000000000000004E-3</v>
+      </c>
+      <c r="S150" s="13">
+        <v>7.1000000000000004E-3</v>
+      </c>
+      <c r="T150" s="13">
+        <v>7.6E-3</v>
+      </c>
+      <c r="U150" s="13">
+        <v>7.6E-3</v>
+      </c>
+      <c r="V150" s="13">
+        <v>7.6E-3</v>
+      </c>
+      <c r="W150" s="13">
+        <v>7.6E-3</v>
+      </c>
+      <c r="X150" s="13">
+        <v>7.6E-3</v>
+      </c>
+      <c r="Y150" s="13">
+        <v>8.6999999999999994E-3</v>
+      </c>
+      <c r="Z150" s="13">
+        <v>8.6999999999999994E-3</v>
+      </c>
+      <c r="AA150" s="13">
+        <v>8.6999999999999994E-3</v>
+      </c>
+      <c r="AB150" s="13">
+        <v>8.6999999999999994E-3</v>
+      </c>
+      <c r="AC150" s="13">
+        <v>8.6999999999999994E-3</v>
       </c>
     </row>
     <row r="151" spans="1:29" x14ac:dyDescent="0.3">
-      <c r="A151" t="s">
+      <c r="A151" s="11" t="s">
         <v>24</v>
       </c>
       <c r="B151" s="8">
         <v>6</v>
       </c>
-      <c r="C151" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="D151" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="E151" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="F151" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="G151" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="H151" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="I151" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="J151" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="K151" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="L151" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="M151" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="N151" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="O151" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="P151" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="Q151" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="R151" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="S151" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="T151" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="U151" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="V151" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="W151" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="X151" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="Y151" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="Z151" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="AA151" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="AB151" s="10">
-        <v>-0.01</v>
-      </c>
-      <c r="AC151" s="10">
-        <v>-0.01</v>
+      <c r="C151" s="13">
+        <v>6.4999999999999997E-3</v>
+      </c>
+      <c r="D151" s="13">
+        <v>6.4999999999999997E-3</v>
+      </c>
+      <c r="E151" s="13">
+        <v>6.4999999999999997E-3</v>
+      </c>
+      <c r="F151" s="13">
+        <v>6.4999999999999997E-3</v>
+      </c>
+      <c r="G151" s="13">
+        <v>6.4999999999999997E-3</v>
+      </c>
+      <c r="H151" s="13">
+        <v>6.4999999999999997E-3</v>
+      </c>
+      <c r="I151" s="13">
+        <v>6.4999999999999997E-3</v>
+      </c>
+      <c r="J151" s="13">
+        <v>7.1000000000000004E-3</v>
+      </c>
+      <c r="K151" s="13">
+        <v>7.1000000000000004E-3</v>
+      </c>
+      <c r="L151" s="13">
+        <v>7.1000000000000004E-3</v>
+      </c>
+      <c r="M151" s="13">
+        <v>7.1000000000000004E-3</v>
+      </c>
+      <c r="N151" s="13">
+        <v>7.1000000000000004E-3</v>
+      </c>
+      <c r="O151" s="13">
+        <v>7.7000000000000002E-3</v>
+      </c>
+      <c r="P151" s="13">
+        <v>7.7000000000000002E-3</v>
+      </c>
+      <c r="Q151" s="13">
+        <v>7.7000000000000002E-3</v>
+      </c>
+      <c r="R151" s="13">
+        <v>7.7000000000000002E-3</v>
+      </c>
+      <c r="S151" s="13">
+        <v>7.7000000000000002E-3</v>
+      </c>
+      <c r="T151" s="13">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="U151" s="13">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="V151" s="13">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="W151" s="13">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="X151" s="13">
+        <v>8.2000000000000007E-3</v>
+      </c>
+      <c r="Y151" s="13">
+        <v>9.9000000000000008E-3</v>
+      </c>
+      <c r="Z151" s="13">
+        <v>9.9000000000000008E-3</v>
+      </c>
+      <c r="AA151" s="13">
+        <v>9.9000000000000008E-3</v>
+      </c>
+      <c r="AB151" s="13">
+        <v>9.9000000000000008E-3</v>
+      </c>
+      <c r="AC151" s="13">
+        <v>9.9000000000000008E-3</v>
       </c>
     </row>
     <row r="152" spans="1:29" x14ac:dyDescent="0.3">

</xml_diff>